<commit_message>
fix bug for python version
</commit_message>
<xml_diff>
--- a/python版/Table/reward.xlsx
+++ b/python版/Table/reward.xlsx
@@ -69,53 +69,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+  <si>
+    <t>item_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>item_number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>道具类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>奖励道具id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>道具个数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>奖励序号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>item_type</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>item_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>item_number</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>道具类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>奖励道具id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>道具个数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>奖励序号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>desc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
+    <t>4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -174,12 +190,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -487,73 +506,73 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="17.625" customWidth="1"/>
-    <col min="3" max="3" width="29.875" customWidth="1"/>
+    <col min="3" max="3" width="59.75" customWidth="1"/>
     <col min="4" max="4" width="27.375" customWidth="1"/>
     <col min="5" max="5" width="25.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>1</v>
       </c>
       <c r="D4" s="2">
@@ -567,8 +586,8 @@
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="1">
-        <v>2</v>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -581,8 +600,8 @@
       <c r="B6">
         <v>3</v>
       </c>
-      <c r="C6">
-        <v>3</v>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D6" s="2">
         <v>510001</v>
@@ -595,169 +614,58 @@
       <c r="B7">
         <v>4</v>
       </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2">
-        <v>10002</v>
-      </c>
-      <c r="E7">
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1">
-        <v>650075</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B9">
-        <v>6</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>500</v>
-      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B10">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>600</v>
-      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B11">
-        <v>8</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11" s="2">
-        <v>510001</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B12">
-        <v>9</v>
-      </c>
-      <c r="C12">
-        <v>4</v>
-      </c>
-      <c r="D12" s="2">
-        <v>10002</v>
-      </c>
-      <c r="E12" s="1">
-        <v>1</v>
-      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B13">
-        <v>10</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
-      <c r="D13" s="1">
-        <v>650075</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B14">
-        <v>11</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1">
-        <v>800</v>
-      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B15">
-        <v>12</v>
-      </c>
-      <c r="C15" s="1">
-        <v>2</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1">
-        <v>1100</v>
-      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B16">
-        <v>13</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16" s="2">
-        <v>510001</v>
-      </c>
-      <c r="E16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B17">
-        <v>14</v>
-      </c>
-      <c r="C17">
-        <v>4</v>
-      </c>
-      <c r="D17" s="2">
-        <v>10002</v>
-      </c>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B18">
-        <v>15</v>
-      </c>
-      <c r="C18">
-        <v>5</v>
-      </c>
-      <c r="D18" s="1">
-        <v>650075</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.15">
+      <c r="D17" s="2"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.15">
+      <c r="D18" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>